<commit_message>
Mppt ved at være der
</commit_message>
<xml_diff>
--- a/Calculations/mppt/mpptkurve.xlsx
+++ b/Calculations/mppt/mpptkurve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Documents\GitHub\ee-projekt\Calculations\mppt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD969EBE-8D6A-4EBB-8F25-924038089182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FDE3A7-A7BD-4E01-991D-7312B018EB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6915D7BA-9E54-48B7-A255-6F7A5307E4CE}"/>
   </bookViews>
@@ -2303,7 +2303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B90F3A9D-DB8F-4F44-BC9C-DD60A333AF75}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="79" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2347,7 +2347,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="F2">
-        <f>E2*D2</f>
+        <f t="shared" ref="F2:F12" si="0">E2*D2</f>
         <v>0.59400000000000008</v>
       </c>
       <c r="G2" s="1">
@@ -2370,7 +2370,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F3">
-        <f>E3*D3</f>
+        <f t="shared" si="0"/>
         <v>0.23399999999999999</v>
       </c>
       <c r="G3" s="1">
@@ -2385,7 +2385,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="F4">
-        <f>E4*D4</f>
+        <f t="shared" si="0"/>
         <v>0.91799999999999993</v>
       </c>
       <c r="G4" s="1">
@@ -2400,7 +2400,7 @@
         <v>0.20200000000000001</v>
       </c>
       <c r="F5">
-        <f>E5*D5</f>
+        <f t="shared" si="0"/>
         <v>3.5148000000000001</v>
       </c>
       <c r="G5" s="1">
@@ -2415,7 +2415,7 @@
         <v>0.308</v>
       </c>
       <c r="F6">
-        <f>E6*D6</f>
+        <f t="shared" si="0"/>
         <v>4.6508000000000003</v>
       </c>
       <c r="G6" s="1">
@@ -2430,7 +2430,7 @@
         <v>0.27700000000000002</v>
       </c>
       <c r="F7">
-        <f>E7*D7</f>
+        <f t="shared" si="0"/>
         <v>3.0054500000000002</v>
       </c>
       <c r="G7" s="1">
@@ -2445,7 +2445,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="F8">
-        <f>E8*D8</f>
+        <f t="shared" si="0"/>
         <v>1.9071000000000002</v>
       </c>
       <c r="G8" s="1">
@@ -2460,7 +2460,7 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="F9">
-        <f>E9*D9</f>
+        <f t="shared" si="0"/>
         <v>1.3024800000000001</v>
       </c>
       <c r="G9" s="1">
@@ -2475,7 +2475,7 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="F10">
-        <f>E10*D10</f>
+        <f t="shared" si="0"/>
         <v>0.95579999999999998</v>
       </c>
       <c r="G10" s="1">
@@ -2490,7 +2490,7 @@
         <v>0.157</v>
       </c>
       <c r="F11">
-        <f>E11*D11</f>
+        <f t="shared" si="0"/>
         <v>0.72062999999999999</v>
       </c>
       <c r="G11" s="1">
@@ -2505,7 +2505,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="F12">
-        <f>E12*D12</f>
+        <f t="shared" si="0"/>
         <v>0.54320000000000002</v>
       </c>
       <c r="G12" s="1">

</xml_diff>